<commit_message>
Ally updates to triggers
</commit_message>
<xml_diff>
--- a/conditions/GlobalConditions.xlsx
+++ b/conditions/GlobalConditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbrau\OneDrive - Lehigh University\Research\By Semester\Summer 2019\NCS\psychopy\build\conditions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alici\Documents\ax-cpt-master\conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{B59A4753-A2E5-42CF-BDA1-C01500AAE50A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D3AF9A16-5687-47BD-B843-096C6CA6AC5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888A29ED-0462-44C8-8A91-F07A17FD5C64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CD37AD06-0CB8-4B7E-832C-CF12F7615E82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD37AD06-0CB8-4B7E-832C-CF12F7615E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
   <si>
     <t>ConditionFile</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>BN</t>
+  </si>
+  <si>
+    <t>cueMarker</t>
+  </si>
+  <si>
+    <t>targetMarker</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81A0B36-F3E1-4742-A528-A1142887D409}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +445,7 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +458,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -466,8 +478,14 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -480,8 +498,14 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -494,8 +518,14 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -508,8 +538,14 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -522,8 +558,14 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -536,8 +578,14 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -550,8 +598,14 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -564,8 +618,14 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -578,8 +638,14 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -592,8 +658,14 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -606,8 +678,14 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -620,8 +698,14 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -634,8 +718,14 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -648,8 +738,14 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -662,8 +758,14 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -676,8 +778,14 @@
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -690,8 +798,14 @@
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -704,8 +818,14 @@
       <c r="D19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -718,8 +838,14 @@
       <c r="D20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -732,8 +858,14 @@
       <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -743,8 +875,14 @@
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -754,8 +892,14 @@
       <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -765,8 +909,14 @@
       <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -775,6 +925,12 @@
       </c>
       <c r="D25">
         <v>1</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added mindwandering catch, practice block, and cleaned up naming
</commit_message>
<xml_diff>
--- a/conditions/GlobalConditions.xlsx
+++ b/conditions/GlobalConditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alici\Documents\ax-cpt-master\conditions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbrau\OneDrive - Lehigh University\Research\By Semester\Summer 2019\NCS\psychopy\build\conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888A29ED-0462-44C8-8A91-F07A17FD5C64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="6_{AF1FAEE7-037D-433E-B935-6C29A12E6327}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{671F3532-0051-4F91-B6D9-3EA1A5223125}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD37AD06-0CB8-4B7E-832C-CF12F7615E82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CD37AD06-0CB8-4B7E-832C-CF12F7615E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="18">
   <si>
     <t>ConditionFile</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>targetMarker</t>
+  </si>
+  <si>
+    <t>conditions/BXList.xlsx</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81A0B36-F3E1-4742-A528-A1142887D409}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -502,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -522,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -542,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -562,7 +566,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -582,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -602,7 +606,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -622,24 +626,24 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>7</v>
@@ -647,19 +651,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -667,19 +671,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -687,19 +691,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>7</v>
@@ -707,10 +711,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -719,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <v>8</v>
@@ -727,10 +731,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -739,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -747,10 +751,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -759,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -767,10 +771,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -779,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -787,10 +791,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -799,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18">
         <v>8</v>
@@ -807,10 +811,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -819,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>8</v>
@@ -827,10 +831,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -839,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20">
         <v>8</v>
@@ -847,10 +851,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -859,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -867,16 +871,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F22">
         <v>9</v>
@@ -884,16 +891,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23">
         <v>9</v>
@@ -901,36 +911,350 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>12</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B40" t="s">
         <v>14</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="F25">
-        <v>10</v>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>6</v>
+      </c>
+      <c r="F40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in additional triggers and adjusted readme
Trigger 13 was added for mindwandering in global conditions, along with a trigger outpush in the mindwanderingcatch routine to send once that routine is activated. Added section to readme folder describing trigger information.
</commit_message>
<xml_diff>
--- a/conditions/GlobalConditions.xlsx
+++ b/conditions/GlobalConditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbrau\OneDrive - Lehigh University\Research\By Semester\Summer 2019\NCS\psychopy\build\conditions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alici\Documents\GitHub\ax-cpt\conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="6_{AF1FAEE7-037D-433E-B935-6C29A12E6327}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{671F3532-0051-4F91-B6D9-3EA1A5223125}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D3104D-8EFF-4B0B-A895-7C8E40178AF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CD37AD06-0CB8-4B7E-832C-CF12F7615E82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD37AD06-0CB8-4B7E-832C-CF12F7615E82}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="19">
   <si>
     <t>ConditionFile</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>conditions/BXList.xlsx</t>
+  </si>
+  <si>
+    <t>wanderingMarker</t>
   </si>
 </sst>
 </file>
@@ -436,20 +439,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81A0B36-F3E1-4742-A528-A1142887D409}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +473,11 @@
       <c r="F1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -488,8 +496,11 @@
       <c r="F2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -508,8 +519,11 @@
       <c r="F3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -528,8 +542,11 @@
       <c r="F4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -548,8 +565,11 @@
       <c r="F5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -568,8 +588,11 @@
       <c r="F6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -588,8 +611,11 @@
       <c r="F7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -608,8 +634,11 @@
       <c r="F8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -628,8 +657,11 @@
       <c r="F9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -648,8 +680,11 @@
       <c r="F10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -668,8 +703,11 @@
       <c r="F11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -688,8 +726,11 @@
       <c r="F12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -708,8 +749,11 @@
       <c r="F13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -728,8 +772,11 @@
       <c r="F14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -748,8 +795,11 @@
       <c r="F15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -768,8 +818,11 @@
       <c r="F16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -788,8 +841,11 @@
       <c r="F17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -808,8 +864,11 @@
       <c r="F18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -828,8 +887,11 @@
       <c r="F19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -848,8 +910,11 @@
       <c r="F20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -868,8 +933,11 @@
       <c r="F21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -888,8 +956,11 @@
       <c r="F22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -908,8 +979,11 @@
       <c r="F23">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -928,8 +1002,11 @@
       <c r="F24">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -948,8 +1025,11 @@
       <c r="F25">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -968,8 +1048,11 @@
       <c r="F26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -988,8 +1071,11 @@
       <c r="F27">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1008,8 +1094,11 @@
       <c r="F28">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -1028,8 +1117,11 @@
       <c r="F29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1048,8 +1140,11 @@
       <c r="F30">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1068,8 +1163,11 @@
       <c r="F31">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1088,8 +1186,11 @@
       <c r="F32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1108,8 +1209,11 @@
       <c r="F33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1128,8 +1232,11 @@
       <c r="F34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1148,8 +1255,11 @@
       <c r="F35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1168,8 +1278,11 @@
       <c r="F36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1188,8 +1301,11 @@
       <c r="F37">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1205,8 +1321,11 @@
       <c r="F38">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -1222,8 +1341,11 @@
       <c r="F39">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -1239,8 +1361,11 @@
       <c r="F40">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -1255,6 +1380,9 @@
       </c>
       <c r="F41">
         <v>12</v>
+      </c>
+      <c r="G41">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>